<commit_message>
before upgrading katalon version
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
+++ b/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\yes breed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B298BA7-0E39-4F1F-ACFD-5BDCD3B5ECFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98637F79-AA2E-434E-ACEB-79B0519E5AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10" windowWidth="19200" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView minimized="1" xWindow="340" yWindow="350" windowWidth="19200" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
to see if bento profile issue gets resolved
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
+++ b/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE8E619-C03D-41E1-8FE3-80AF03AE98A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8954C1-4A53-4EBC-8C22-F0CAA2D7EC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,23 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE samp.summarized_sample_type IN ["Normal Tissue"]  
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
  MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
@@ -99,8 +115,7 @@
         coalesce(f.file_format, '') AS `Format`,
         coalesce(f.file_size, '') AS `Size`,
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.disease_term,'') AS Diagnosis  </t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -119,55 +134,8 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-      WHERE (size([]) = 0 OR s.clinical_study_designation IN [])
-        AND (s.study_disposition = 'Unrestricted')
-        AND (size([]) = 0 OR s.clinical_study_type IN [])
-        AND (size([]) = 0 OR demo.breed IN [])
-        AND (size([]) = 0 OR demo.sex IN [])
-        AND (size([]) = 0 OR demo.neutered_indicator IN [])
-        AND (size([]) = 0 OR diag.disease_term IN [])
-        AND (size([]) = 0 OR diag.primary_disease_site IN [])
-        AND (size([]) = 0 OR diag.stage_of_disease IN [])
-        AND (size([]) = 0 OR diag.best_response IN [])
-    OPTIONAL MATCH (c)--&gt;(co:cohort)
-    OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-    OPTIONAL MATCH (f)--&gt;(parent)
-    OPTIONAL MATCH (samp:sample)--&gt;(c)
-    OPTIONAL MATCH (samp)&lt;--(al:aliquot)
-    WITH DISTINCT c AS c, p, s, co, demo, diag, f, parent, samp, al
-      WHERE (size(['Normal Tissue']) = 0 OR samp.summarized_sample_type IN ['Normal Tissue'])
-        AND (size([]) = 0 OR samp.specific_sample_pathology IN [])
-        AND (size([]) = 0 OR samp.sample_site IN [])
-        AND (size([]) = 0 OR head(labels(parent)) IN [])
-        AND (size([]) = 0 OR f.file_type IN [])
-        AND (size([]) = 0 OR f.file_format IN [])
-    WITH c.case_id AS case_id,
-         s.clinical_study_designation AS study_code,
-         s.clinical_study_type AS study_type,
-         co.cohort_description AS cohort,
-         demo.breed AS breed,
-         diag.disease_term AS diagnosis,
-         diag.stage_of_disease AS stage_of_disease,
-         diag.primary_disease_site AS disease_site,
-         demo.patient_age_at_enrollment AS age,
-         demo.sex AS sex,
-         demo.neutered_indicator AS neutered_status,
-         demo.weight AS weight,
-         diag.best_response AS response_to_treatment,
-         samp.sample_id AS sample_id,
-         f.uuid AS file_id,
-         al
-    RETURN
-COUNT(DISTINCT file_id) as number_of_files,
-COUNT(DISTINCT sample_id) as number_of_sample,
-COUNT(DISTINCT case_id) as number_of_cases,
-COUNT(DISTINCT study_code) as number_of_study,
-COUNT(DISTINCT al) as number_of_aliquot
-    </t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -539,20 +507,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -569,15 +537,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -586,7 +554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -594,7 +562,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -603,15 +571,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added ICDC_JenkinsTest to run in jenkins
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
+++ b/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8954C1-4A53-4EBC-8C22-F0CAA2D7EC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C39D6-450B-4E89-8BD6-A8111215430E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ctdc gender male script with db in qa
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
+++ b/InputFiles/TC03_Canine_Filter_SampleType-NormalTissue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\TestInputFiles_Sowjanya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Scripts to correct\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ADB9FD-800B-4AC8-8A13-3E7DD2EA01EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31940812-30D4-4ADD-872E-6249229A58EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,40 @@
     count(distinct samp) AS Samples,
     count(distinct f) AS `Case Files`,
     count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+ MATCH (samp:sample)--&gt;(c) 
+ WHERE samp.summarized_sample_type IN ["Normal Tissue"]  
+WITH DISTINCT f, parent, c, demo, diag, s
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis</t>
   </si>
   <si>
     <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
@@ -128,40 +162,6 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c) 
- WHERE samp.summarized_sample_type IN ["Normal Tissue"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp:sample)
-WITH
-        f, parent, c, demo, diag, s, samp,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH
-        f, parent, c, demo, diag, s, samp,
-        f.file_size /(1024^i) AS value, 
-        10^precision AS factor,
-        units[i] as unit
-WITH    
-        f, parent, c, demo, diag, s, samp, unit,
-        round(factor * value)/factor AS size
-RETURN 
-        coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-        coalesce(samp.sample_id, '') AS `Sample ID`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed ,
-        coalesce(diag.disease_term,'') AS Diagnosis</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 MATCH (samp:sample)--&gt;(c) 
@@ -178,7 +178,7 @@
        CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
        coalesce(demo.sex, '') AS Sex,
        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-          coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
        coalesce(diag.best_response, '') AS `Response to Treatment`,
        coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
@@ -556,16 +556,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" customWidth="1"/>
-    <col min="3" max="3" width="75.7109375" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.7265625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -599,12 +599,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -616,12 +616,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -633,12 +633,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>

</xml_diff>